<commit_message>
Assignment 5 - V5 (TASK 1 AND 2 FINISCHED)
</commit_message>
<xml_diff>
--- a/Assignment 5/DecisionTreesFiguresHelp(Dont,send).xlsx
+++ b/Assignment 5/DecisionTreesFiguresHelp(Dont,send).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ae9f155d4a90194/cesar/extranjero/Alemania BWU/Uni Weimar/2 semester/ML/Assignments/Assignment 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{F2866D70-6B44-4A4E-9B4D-D71740DE0760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C690788A-52BD-476D-BCEC-3100374029EB}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="8_{F2866D70-6B44-4A4E-9B4D-D71740DE0760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{365270AD-59FE-402C-B7FC-DB9433D02464}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="3816" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{F488649C-151F-43A5-9718-3DB8384D514C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>A XOR B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A or (B and C)</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>(A and B) or ( C and D)</t>
   </si>
 </sst>
 </file>
@@ -110,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,6 +131,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2144,7 +2159,3615 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C3B1E6-B9DC-4BA7-8980-5041B87BAA3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5120640" y="7802880"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>167164</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E3C6B03-7D60-48A2-8FA0-D059EF5B3359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4312920" y="8381743"/>
+          <a:ext cx="921544" cy="716537"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83344</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>137417</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>357664</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>45977</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{457EE8CC-0328-4F12-B25D-F3E94CFE9F40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4541044" y="8549897"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA69FC9D-A491-45B6-933D-2EF10C1C12BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3985260" y="9098280"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>TRUE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>107156</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9393F0AC-64E5-4926-8CA6-05F731DBD7BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="5"/>
+          <a:endCxn id="34" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784056" y="8381743"/>
+          <a:ext cx="776764" cy="670817"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>464344</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>84077</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>129064</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>175517</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="TextBox 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E17F309-6422-4B27-B3B3-CCDE434FE14C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6141244" y="8496557"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Oval 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4601CEB-9A57-43F7-9461-5FB28EF798AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6172200" y="9052560"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="Oval 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61FF24D6-0BB5-47D7-8A0D-2FDDACC7300E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5265420" y="10287000"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>121663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609124</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Connector 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DBAE1CF-BB48-4CC8-A2FC-23305132238C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="3"/>
+          <a:endCxn id="45" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5654040" y="9631423"/>
+          <a:ext cx="631984" cy="655577"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>136684</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>61217</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>411004</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152657</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="TextBox 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{229ADDA7-814B-4ED8-940C-77F3304E082A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5813584" y="9753857"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Rectangle 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7CE3FBE-7FCF-4880-8DA6-85274375743E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7048500" y="10386060"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>FALSE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>549116</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>121663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Straight Connector 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27EF129F-E22D-40A9-A790-E6BB87C54B3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="5"/>
+          <a:endCxn id="59" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6835616" y="9631423"/>
+          <a:ext cx="540544" cy="754637"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>167164</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>68837</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>441484</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>160277</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="TextBox 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2791A35-1A7B-4D39-89B6-4F6B14689BFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7063264" y="9761477"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>75943</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>311944</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Straight Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2596C54-3C2D-4509-A15C-B83AC0851675}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="3"/>
+          <a:endCxn id="73" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4869180" y="10865863"/>
+          <a:ext cx="510064" cy="716537"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>487204</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>145037</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>151924</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>53597</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="TextBox 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703C330B-8479-47E9-AEBC-5716F3A3382B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4944904" y="10934957"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>251936</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>75943</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Straight Connector 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4370C4B4-A0EA-400B-AACC-9E0FBAA71BC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="5"/>
+          <a:endCxn id="75" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5928836" y="10865863"/>
+          <a:ext cx="334804" cy="731777"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Rectangle 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{833449FB-35E4-4CB7-ABE3-861A74B6FA2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4541520" y="11582400"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>TRUE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="Rectangle 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B34162E7-3FC3-484E-ADF1-F5C36887CA98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5935980" y="11597640"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>FALSE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="TextBox 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5691EE65-7DB5-4FF4-B077-3F0FAFA6FC39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5996940" y="10942320"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="Oval 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4C6A07E-B46E-4B7A-A391-0EAFE930554C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6896100" y="12595860"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Oval 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2650A483-9139-4E77-9648-E563C3CCA05D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5250180" y="13540740"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Oval 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91ABCD31-E41E-488D-8D96-CF14ECE8D25B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8709660" y="13601700"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="82" name="Oval 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1DA60A5-C540-4613-9FB2-AEA6A2AEEDB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195060" y="14668500"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Oval 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC279818-859A-4117-92D3-522DA469672E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8100060" y="14881860"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>D</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="Oval 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B6837B-96E8-41EB-AAE2-715D59F701EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5242560" y="15841980"/>
+          <a:ext cx="777240" cy="678180"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" kern="1200"/>
+            <a:t>D</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>396716</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>106937</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Straight Connector 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5F56E5B-FF81-483A-83E1-2DC27D50B78F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="79" idx="4"/>
+          <a:endCxn id="80" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5913596" y="13274040"/>
+          <a:ext cx="1371124" cy="366017"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>258604</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>167897</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="Straight Connector 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DF9D002-E2A7-4C02-8F2C-B7C818D3D0F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="79" idx="4"/>
+          <a:endCxn id="81" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7284720" y="13274040"/>
+          <a:ext cx="1538764" cy="426977"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>396716</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>37843</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Straight Connector 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693BF299-DF4C-450C-886E-9B192705CD0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="80" idx="5"/>
+          <a:endCxn id="82" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5913596" y="14119603"/>
+          <a:ext cx="670084" cy="548897"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>98803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>258604</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="94" name="Straight Connector 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C599BC58-B772-4F9C-A075-1C0EA7D66320}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="81" idx="3"/>
+          <a:endCxn id="83" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8488680" y="14180563"/>
+          <a:ext cx="334804" cy="701297"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="Straight Connector 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5FDDCDA-A1C2-4934-9638-7F8051BC855B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="82" idx="4"/>
+          <a:endCxn id="84" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5631180" y="15346680"/>
+          <a:ext cx="952500" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="TextBox 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4CC01ED-D40A-47B3-9838-1C06C6D91942}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6256020" y="13213080"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="TextBox 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D793FE07-7502-48CA-B5BE-C2CEE3208B46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5753100" y="15407640"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="TextBox 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F07789E-4B0D-4A05-8BE2-CC6D87C9F138}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5097780" y="16588740"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="Straight Connector 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD660A50-F3DB-4286-B184-393493FCADCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="84" idx="4"/>
+          <a:endCxn id="113" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5090160" y="16520160"/>
+          <a:ext cx="541020" cy="487680"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="113" name="Rectangle 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B8C63E-FEA3-4483-BE0E-0F492B71604D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="17007840"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>TRUE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="116" name="Rectangle 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F6AB952-EDA3-4B9F-BC4D-8291D6E21587}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5829300" y="17015460"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>FALSE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="117" name="Straight Connector 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{601DE893-524C-40A9-BEF4-9790D4F35B69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="84" idx="4"/>
+          <a:endCxn id="116" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5631180" y="16520160"/>
+          <a:ext cx="525780" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="121" name="TextBox 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB20D7E-5EA2-44D8-80F0-5FBC59A9240B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5882640" y="16550640"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="122" name="Straight Connector 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5838640F-E0A3-440D-9CA3-C9FF225DD736}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="82" idx="4"/>
+          <a:endCxn id="125" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6583680" y="15346680"/>
+          <a:ext cx="693420" cy="510540"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="125" name="Rectangle 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDCBBCC8-BAB7-46FE-AFE0-98B3663E6633}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6949440" y="15857220"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>FALSE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="TextBox 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34375BB8-EE9E-41CB-AF51-7C36B6B7780C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6911340" y="15377160"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="136" name="Rectangle 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDFA44B9-203C-434C-B6FB-344D03ECCCFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4663440" y="14569440"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>TRUE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>37843</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>456724</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="137" name="Straight Connector 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777056F6-DD4D-4DE2-BD6B-2C4E7393CE6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="80" idx="3"/>
+          <a:endCxn id="136" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4991100" y="14119603"/>
+          <a:ext cx="372904" cy="449837"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="141" name="TextBox 140">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF53D17-A74D-4F65-B630-7FC91783BF18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4960620" y="14104620"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="142" name="TextBox 141">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C143E86-5928-4352-96F4-BF36CF228E90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6004560" y="14066520"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="147" name="TextBox 146">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2392DD57-A041-4E00-8B8A-E1446FF6FC7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8237220" y="13243560"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="148" name="TextBox 147">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56772C25-9113-4F55-B24C-EC020BC0D5E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9326880" y="14417040"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="149" name="TextBox 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6B7A6EB-BE16-4FC1-9503-89AE026B115F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8389620" y="14378940"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>198596</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>98803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="150" name="Straight Connector 149">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5BDD3B2-6947-497D-A3A8-3B1C32547C0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="81" idx="5"/>
+          <a:endCxn id="153" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9373076" y="14180563"/>
+          <a:ext cx="555784" cy="762257"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="153" name="Rectangle 152">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2925E3BB-E89C-4CCA-9694-A262F3A2E8E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9601200" y="14942820"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>FALSE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="180" name="Rectangle 179">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D81351-BB56-4DA2-A1AD-3332E3327BB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7802880" y="15841980"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>TRUE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="181" name="Rectangle 180">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59987FBF-CC94-4C74-A590-47804B566637}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8663940" y="15841980"/>
+          <a:ext cx="655320" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>FALSE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>98803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>258604</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="182" name="Straight Connector 181">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCB9113-607A-4C68-89DE-FA4B061A3B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="83" idx="3"/>
+          <a:endCxn id="180" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8130540" y="15460723"/>
+          <a:ext cx="83344" cy="381257"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>198596</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>98803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="185" name="Straight Connector 184">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F412247-8C97-4163-A9AD-09782F673946}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="83" idx="5"/>
+          <a:endCxn id="181" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8763476" y="15460723"/>
+          <a:ext cx="228124" cy="381257"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="190" name="TextBox 189">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62AB0AE3-53EC-47C0-8DA1-8411295AB20C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7940040" y="15468600"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="191" name="TextBox 190">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4790E4-772B-4968-A844-2D3BB55FB92E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808720" y="15445740"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2464,16 +6087,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16F88D0-CB3B-41C6-9F29-BDF6B96550D7}">
-  <dimension ref="C3:P507"/>
+  <dimension ref="A3:P507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.3">
@@ -2926,7 +6549,7 @@
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -2938,7 +6561,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2950,7 +6573,7 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2962,7 +6585,7 @@
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2974,7 +6597,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -2986,7 +6609,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2998,7 +6621,7 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -3010,7 +6633,7 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -3022,7 +6645,7 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -3034,7 +6657,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -3046,7 +6669,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -3058,7 +6681,19 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3070,7 +6705,19 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0</v>
+      </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3082,7 +6729,19 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0</v>
+      </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3094,7 +6753,19 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B47" s="4">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0</v>
+      </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -3106,7 +6777,19 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B48" s="4">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4">
+        <v>1</v>
+      </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -3118,7 +6801,19 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
     </row>
-    <row r="49" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -3130,7 +6825,19 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -3142,7 +6849,19 @@
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -3154,7 +6873,19 @@
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -3166,7 +6897,7 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
     </row>
-    <row r="53" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -3178,7 +6909,7 @@
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
     </row>
-    <row r="54" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -3190,7 +6921,7 @@
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
     </row>
-    <row r="55" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -3202,7 +6933,7 @@
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
     </row>
-    <row r="56" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -3214,7 +6945,7 @@
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
     </row>
-    <row r="57" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -3226,7 +6957,7 @@
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
     </row>
-    <row r="58" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -3238,7 +6969,7 @@
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
     </row>
-    <row r="59" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
@@ -3250,7 +6981,7 @@
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
     </row>
-    <row r="60" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
@@ -3262,7 +6993,7 @@
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
     </row>
-    <row r="61" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -3274,7 +7005,7 @@
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
     </row>
-    <row r="62" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -3286,7 +7017,7 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
     </row>
-    <row r="63" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -3298,7 +7029,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
@@ -3310,7 +7041,7 @@
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
     </row>
-    <row r="65" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -3322,7 +7053,7 @@
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
     </row>
-    <row r="66" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -3334,7 +7065,7 @@
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
     </row>
-    <row r="67" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
@@ -3346,7 +7077,7 @@
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
     </row>
-    <row r="68" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -3358,7 +7089,7 @@
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
     </row>
-    <row r="69" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -3370,7 +7101,22 @@
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
     </row>
-    <row r="70" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -3382,7 +7128,22 @@
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
     </row>
-    <row r="71" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>0</v>
+      </c>
+      <c r="B71" s="4">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0</v>
+      </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -3394,7 +7155,22 @@
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
     </row>
-    <row r="72" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>0</v>
+      </c>
+      <c r="B72" s="4">
+        <v>0</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0</v>
+      </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3406,7 +7182,22 @@
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
     </row>
-    <row r="73" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>0</v>
+      </c>
+      <c r="B73" s="4">
+        <v>0</v>
+      </c>
+      <c r="C73" s="4">
+        <v>1</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0</v>
+      </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3418,7 +7209,22 @@
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
     </row>
-    <row r="74" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A74" s="4">
+        <v>0</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0</v>
+      </c>
+      <c r="C74" s="4">
+        <v>1</v>
+      </c>
+      <c r="D74" s="4">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -3430,7 +7236,22 @@
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
     </row>
-    <row r="75" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75" s="4">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -3442,7 +7263,22 @@
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
     </row>
-    <row r="76" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A76" s="4">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -3454,7 +7290,22 @@
       <c r="O76" s="3"/>
       <c r="P76" s="3"/>
     </row>
-    <row r="77" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A77" s="4">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -3466,7 +7317,22 @@
       <c r="O77" s="3"/>
       <c r="P77" s="3"/>
     </row>
-    <row r="78" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A78" s="4">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -3478,7 +7344,22 @@
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
     </row>
-    <row r="79" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A79" s="4">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0</v>
+      </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -3490,7 +7371,22 @@
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
     </row>
-    <row r="80" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80" s="4">
+        <v>1</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3502,7 +7398,22 @@
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
     </row>
-    <row r="81" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A81" s="4">
+        <v>1</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -3514,7 +7425,22 @@
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
     </row>
-    <row r="82" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A82" s="4">
+        <v>1</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -3526,7 +7452,22 @@
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
     </row>
-    <row r="83" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A83" s="4">
+        <v>1</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3538,7 +7479,22 @@
       <c r="O83" s="3"/>
       <c r="P83" s="3"/>
     </row>
-    <row r="84" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A84" s="4">
+        <v>1</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -3550,7 +7506,22 @@
       <c r="O84" s="3"/>
       <c r="P84" s="3"/>
     </row>
-    <row r="85" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A85" s="4">
+        <v>1</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -3562,7 +7533,22 @@
       <c r="O85" s="3"/>
       <c r="P85" s="3"/>
     </row>
-    <row r="86" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A86" s="4">
+        <v>1</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -3574,7 +7560,7 @@
       <c r="O86" s="3"/>
       <c r="P86" s="3"/>
     </row>
-    <row r="87" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3586,7 +7572,7 @@
       <c r="O87" s="3"/>
       <c r="P87" s="3"/>
     </row>
-    <row r="88" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3598,7 +7584,7 @@
       <c r="O88" s="3"/>
       <c r="P88" s="3"/>
     </row>
-    <row r="89" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3610,7 +7596,7 @@
       <c r="O89" s="3"/>
       <c r="P89" s="3"/>
     </row>
-    <row r="90" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -3622,7 +7608,7 @@
       <c r="O90" s="3"/>
       <c r="P90" s="3"/>
     </row>
-    <row r="91" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3634,7 +7620,7 @@
       <c r="O91" s="3"/>
       <c r="P91" s="3"/>
     </row>
-    <row r="92" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -3646,7 +7632,7 @@
       <c r="O92" s="3"/>
       <c r="P92" s="3"/>
     </row>
-    <row r="93" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -3658,7 +7644,7 @@
       <c r="O93" s="3"/>
       <c r="P93" s="3"/>
     </row>
-    <row r="94" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -3670,7 +7656,7 @@
       <c r="O94" s="3"/>
       <c r="P94" s="3"/>
     </row>
-    <row r="95" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -3682,7 +7668,7 @@
       <c r="O95" s="3"/>
       <c r="P95" s="3"/>
     </row>
-    <row r="96" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>

</xml_diff>